<commit_message>
Fixed ETM reports backlog
</commit_message>
<xml_diff>
--- a/public/abcd/ETM Audit Status Report.xlsx
+++ b/public/abcd/ETM Audit Status Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>QixTix | Automated Fare Collection System</t>
   </si>
@@ -23,13 +23,13 @@
     <t>ETM Audit Status Report</t>
   </si>
   <si>
-    <t>Depot : BALEWADI</t>
-  </si>
-  <si>
-    <t>From : 01-09-2018</t>
-  </si>
-  <si>
-    <t>To : 12-03-2019</t>
+    <t>Depot : opiant</t>
+  </si>
+  <si>
+    <t>From : 01-10-2018</t>
+  </si>
+  <si>
+    <t>To : 24-04-2019</t>
   </si>
   <si>
     <t>Shift : All</t>
@@ -62,49 +62,43 @@
     <t>Vehicle No.</t>
   </si>
   <si>
-    <t>Handed Over To</t>
-  </si>
-  <si>
     <t>Audited</t>
   </si>
   <si>
-    <t>13-12-2018 20:30:41</t>
-  </si>
-  <si>
-    <t>V2-1-I-Morning</t>
-  </si>
-  <si>
-    <t>13-12-2018 20:52:04</t>
-  </si>
-  <si>
-    <t>A.S. Salvi(802711)</t>
-  </si>
-  <si>
-    <t>MH02CD7033</t>
+    <t>Audited By</t>
+  </si>
+  <si>
+    <t>Cash Remitted By</t>
+  </si>
+  <si>
+    <t>O2-2-1-Afternoon</t>
+  </si>
+  <si>
+    <t>subhash(123123)</t>
+  </si>
+  <si>
+    <t>RJ27BE4554</t>
   </si>
   <si>
     <t>Un-audited</t>
   </si>
   <si>
-    <t>13-12-2018 19:33:07</t>
-  </si>
-  <si>
-    <t>13-12-2018 20:29:28</t>
-  </si>
-  <si>
-    <t>13-12-2018 18:31:50</t>
-  </si>
-  <si>
-    <t>13-12-2018 19:29:18</t>
-  </si>
-  <si>
-    <t>MH01AB7033</t>
+    <t>Apurv(242424)</t>
+  </si>
+  <si>
+    <t>up13ba2296</t>
+  </si>
+  <si>
+    <t>01-03-2019 15:34:34</t>
+  </si>
+  <si>
+    <t>Satya</t>
   </si>
   <si>
     <t>Print taken by : Satya</t>
   </si>
   <si>
-    <t>Print taken at : 12-03-2019 13:05:39</t>
+    <t>Print taken at : 24-04-2019 14:52:42</t>
   </si>
 </sst>
 </file>
@@ -529,10 +523,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,6 +543,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1"/>
@@ -560,6 +555,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
@@ -573,6 +569,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
@@ -604,6 +601,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
@@ -633,31 +631,28 @@
       <c r="I7" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="J7" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>2147483647</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
+        <v>55237734</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -665,25 +660,19 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>2147483647</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
+        <v>55237733</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
       <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>6495</v>
-      </c>
-      <c r="I9" t="s">
         <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -691,49 +680,72 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>2147483647</v>
+        <v>55237734</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>55237734</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F13" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="I10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:I2"/>
-    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="C1:J2"/>
+    <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="F13:J13"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>